<commit_message>
fix ga, lstm, naive
</commit_message>
<xml_diff>
--- a/output/ga_results/ga_report.xlsx
+++ b/output/ga_results/ga_report.xlsx
@@ -956,13 +956,13 @@
         <v>0</v>
       </c>
       <c r="BI2" t="n">
-        <v>1</v>
+        <v>0.8975343106629416</v>
       </c>
       <c r="BJ2" t="n">
-        <v>1</v>
+        <v>0.8975343106629416</v>
       </c>
       <c r="BK2" t="n">
-        <v>100</v>
+        <v>89.75</v>
       </c>
       <c r="BL2" t="inlineStr">
         <is>
@@ -970,7 +970,7 @@
         </is>
       </c>
       <c r="BM2" t="n">
-        <v>5.98699170355107</v>
+        <v>5.782504626231201</v>
       </c>
     </row>
     <row r="3">
@@ -1162,13 +1162,13 @@
         <v>0</v>
       </c>
       <c r="BI3" t="n">
-        <v>0.9322687188161658</v>
+        <v>0.9259739153066067</v>
       </c>
       <c r="BJ3" t="n">
-        <v>0.9322687188161658</v>
+        <v>0.9259739153066067</v>
       </c>
       <c r="BK3" t="n">
-        <v>93.23</v>
+        <v>92.59999999999999</v>
       </c>
       <c r="BL3" t="inlineStr">
         <is>
@@ -1176,7 +1176,7 @@
         </is>
       </c>
       <c r="BM3" t="n">
-        <v>5.851822830711569</v>
+        <v>5.839260518582497</v>
       </c>
     </row>
     <row r="4">
@@ -1366,13 +1366,13 @@
         <v>0.6928203230275504</v>
       </c>
       <c r="BI4" t="n">
-        <v>0.0001</v>
+        <v>0.251511556867749</v>
       </c>
       <c r="BJ4" t="n">
-        <v>0.0001</v>
+        <v>0.251511556867749</v>
       </c>
       <c r="BK4" t="n">
-        <v>0.01</v>
+        <v>25.15</v>
       </c>
       <c r="BL4" t="inlineStr">
         <is>
@@ -1572,13 +1572,13 @@
         <v>0.6928203230275506</v>
       </c>
       <c r="BI5" t="n">
-        <v>0.06516278616970395</v>
+        <v>0.0001</v>
       </c>
       <c r="BJ5" t="n">
-        <v>0.06516278616970395</v>
+        <v>0.0001</v>
       </c>
       <c r="BK5" t="n">
-        <v>6.52</v>
+        <v>0.01</v>
       </c>
       <c r="BL5" t="inlineStr">
         <is>
@@ -1778,13 +1778,13 @@
         <v>0.6328506932918696</v>
       </c>
       <c r="BI6" t="n">
-        <v>0.8660260372187892</v>
+        <v>0.8548821979343928</v>
       </c>
       <c r="BJ6" t="n">
-        <v>0.8660260372187892</v>
+        <v>0.8548821979343928</v>
       </c>
       <c r="BK6" t="n">
-        <v>86.59999999999999</v>
+        <v>85.48999999999999</v>
       </c>
       <c r="BL6" t="inlineStr">
         <is>
@@ -1792,7 +1792,7 @@
         </is>
       </c>
       <c r="BM6" t="n">
-        <v>3.993922385944024</v>
+        <v>3.978392998351124</v>
       </c>
     </row>
     <row r="7">
@@ -1983,13 +1983,13 @@
         <v>0.584807660688538</v>
       </c>
       <c r="BI7" t="n">
-        <v>0.7804556995701294</v>
+        <v>0.7395082100789241</v>
       </c>
       <c r="BJ7" t="n">
-        <v>0.7804556995701294</v>
+        <v>0.7395082100789241</v>
       </c>
       <c r="BK7" t="n">
-        <v>78.05</v>
+        <v>73.95</v>
       </c>
       <c r="BL7" t="inlineStr">
         <is>
@@ -1997,7 +1997,7 @@
         </is>
       </c>
       <c r="BM7" t="n">
-        <v>3.874676683822134</v>
+        <v>3.817614712715328</v>
       </c>
     </row>
     <row r="8">
@@ -2189,13 +2189,13 @@
         <v>0.5457628998540878</v>
       </c>
       <c r="BI8" t="n">
-        <v>0.955342012406263</v>
+        <v>0.761243694776387</v>
       </c>
       <c r="BJ8" t="n">
-        <v>0.955342012406263</v>
+        <v>0.761243694776387</v>
       </c>
       <c r="BK8" t="n">
-        <v>95.53</v>
+        <v>76.12</v>
       </c>
       <c r="BL8" t="inlineStr">
         <is>
@@ -2203,7 +2203,7 @@
         </is>
       </c>
       <c r="BM8" t="n">
-        <v>4.118387784405595</v>
+        <v>3.847903983564655</v>
       </c>
     </row>
     <row r="9">
@@ -2394,13 +2394,13 @@
         <v>0.4217311262607299</v>
       </c>
       <c r="BI9" t="n">
-        <v>0.8002671504870114</v>
+        <v>0.8626015846940868</v>
       </c>
       <c r="BJ9" t="n">
-        <v>0.8002671504870114</v>
+        <v>0.8626015846940868</v>
       </c>
       <c r="BK9" t="n">
-        <v>80.03</v>
+        <v>86.26000000000001</v>
       </c>
       <c r="BL9" t="inlineStr">
         <is>
@@ -2408,7 +2408,7 @@
         </is>
       </c>
       <c r="BM9" t="n">
-        <v>3.902284736326692</v>
+        <v>3.989150273820687</v>
       </c>
     </row>
     <row r="10">
@@ -2601,13 +2601,13 @@
         <v>0.4777177887773147</v>
       </c>
       <c r="BI10" t="n">
-        <v>0.8449251380807483</v>
+        <v>0.8342082463533553</v>
       </c>
       <c r="BJ10" t="n">
-        <v>0.8449251380807483</v>
+        <v>0.8342082463533553</v>
       </c>
       <c r="BK10" t="n">
-        <v>84.48999999999999</v>
+        <v>83.42</v>
       </c>
       <c r="BL10" t="inlineStr">
         <is>
@@ -2615,7 +2615,7 @@
         </is>
       </c>
       <c r="BM10" t="n">
-        <v>5.933329653520449</v>
+        <v>5.910978678224625</v>
       </c>
     </row>
     <row r="11">
@@ -2807,13 +2807,13 @@
         <v>0.6026726190182244</v>
       </c>
       <c r="BI11" t="n">
-        <v>0.75847981791585</v>
+        <v>0.7139596494856451</v>
       </c>
       <c r="BJ11" t="n">
-        <v>0.75847981791585</v>
+        <v>0.7139596494856451</v>
       </c>
       <c r="BK11" t="n">
-        <v>75.84999999999999</v>
+        <v>71.40000000000001</v>
       </c>
       <c r="BL11" t="inlineStr">
         <is>
@@ -2821,7 +2821,7 @@
         </is>
       </c>
       <c r="BM11" t="n">
-        <v>5.753040698047799</v>
+        <v>5.660190157978803</v>
       </c>
     </row>
     <row r="12">
@@ -3013,13 +3013,13 @@
         <v>0.5855400437691201</v>
       </c>
       <c r="BI12" t="n">
-        <v>0.8233404440771093</v>
+        <v>0.9199718003314667</v>
       </c>
       <c r="BJ12" t="n">
-        <v>0.8233404440771093</v>
+        <v>0.9199718003314667</v>
       </c>
       <c r="BK12" t="n">
-        <v>82.33</v>
+        <v>92</v>
       </c>
       <c r="BL12" t="inlineStr">
         <is>
@@ -3027,7 +3027,7 @@
         </is>
       </c>
       <c r="BM12" t="n">
-        <v>3.934438297595932</v>
+        <v>4.069097973368776</v>
       </c>
     </row>
     <row r="13">
@@ -3220,13 +3220,13 @@
         <v>0.6244997998398401</v>
       </c>
       <c r="BI13" t="n">
-        <v>0.6775390761516846</v>
+        <v>0.6800692474526799</v>
       </c>
       <c r="BJ13" t="n">
-        <v>0.6775390761516846</v>
+        <v>0.6800692474526799</v>
       </c>
       <c r="BK13" t="n">
-        <v>67.75</v>
+        <v>68.01000000000001</v>
       </c>
       <c r="BL13" t="inlineStr">
         <is>
@@ -3234,7 +3234,7 @@
         </is>
       </c>
       <c r="BM13" t="n">
-        <v>3.296437275116855</v>
+        <v>3.299552281378881</v>
       </c>
     </row>
     <row r="14">
@@ -3632,13 +3632,13 @@
         <v>0.707359274242687</v>
       </c>
       <c r="BI15" t="n">
-        <v>0.5635407836991131</v>
+        <v>0.5563274019391721</v>
       </c>
       <c r="BJ15" t="n">
-        <v>0.5635407836991131</v>
+        <v>0.5563274019391721</v>
       </c>
       <c r="BK15" t="n">
-        <v>56.35</v>
+        <v>55.63</v>
       </c>
       <c r="BL15" t="inlineStr">
         <is>
@@ -3646,7 +3646,7 @@
         </is>
       </c>
       <c r="BM15" t="n">
-        <v>5.115965801240466</v>
+        <v>5.101570315656695</v>
       </c>
     </row>
     <row r="16">
@@ -3838,13 +3838,13 @@
         <v>0.6579187965525378</v>
       </c>
       <c r="BI16" t="n">
-        <v>0.6546605430963264</v>
+        <v>0.6068919016003881</v>
       </c>
       <c r="BJ16" t="n">
-        <v>0.6546605430963264</v>
+        <v>0.6068919016003881</v>
       </c>
       <c r="BK16" t="n">
-        <v>65.47</v>
+        <v>60.69</v>
       </c>
       <c r="BL16" t="inlineStr">
         <is>
@@ -3852,7 +3852,7 @@
         </is>
       </c>
       <c r="BM16" t="n">
-        <v>5.297810215754027</v>
+        <v>5.202480062311999</v>
       </c>
     </row>
     <row r="17">
@@ -4044,21 +4044,21 @@
         <v>0.6447590912226693</v>
       </c>
       <c r="BI17" t="n">
-        <v>0.4482987068515692</v>
+        <v>0.7435041105165291</v>
       </c>
       <c r="BJ17" t="n">
-        <v>0.4482987068515692</v>
+        <v>0.7435041105165291</v>
       </c>
       <c r="BK17" t="n">
-        <v>44.83</v>
+        <v>74.34999999999999</v>
       </c>
       <c r="BL17" t="inlineStr">
         <is>
-          <t>Aman</t>
+          <t>Terdampak</t>
         </is>
       </c>
       <c r="BM17" t="n">
-        <v>4.885981348578386</v>
+        <v>5.475112116106906</v>
       </c>
     </row>
     <row r="18">
@@ -4250,13 +4250,13 @@
         <v>0.630476010645922</v>
       </c>
       <c r="BI18" t="n">
-        <v>0.3884902514512227</v>
+        <v>0.5677565934530615</v>
       </c>
       <c r="BJ18" t="n">
-        <v>0.3884902514512227</v>
+        <v>0.5677565934530615</v>
       </c>
       <c r="BK18" t="n">
-        <v>38.85</v>
+        <v>56.78</v>
       </c>
       <c r="BL18" t="inlineStr">
         <is>
@@ -4264,7 +4264,7 @@
         </is>
       </c>
       <c r="BM18" t="n">
-        <v>4.766623773150359</v>
+        <v>5.124379140580679</v>
       </c>
     </row>
     <row r="19">
@@ -4456,13 +4456,13 @@
         <v>0.6026726190182213</v>
       </c>
       <c r="BI19" t="n">
-        <v>0.955342012406263</v>
+        <v>1</v>
       </c>
       <c r="BJ19" t="n">
-        <v>0.955342012406263</v>
+        <v>1</v>
       </c>
       <c r="BK19" t="n">
-        <v>95.53</v>
+        <v>100</v>
       </c>
       <c r="BL19" t="inlineStr">
         <is>
@@ -4470,7 +4470,7 @@
         </is>
       </c>
       <c r="BM19" t="n">
-        <v>4.36338906393521</v>
+        <v>4.429323962118182</v>
       </c>
     </row>
     <row r="20">
@@ -4662,13 +4662,13 @@
         <v>0.5185832348124723</v>
       </c>
       <c r="BI20" t="n">
-        <v>0.9322687188161658</v>
+        <v>0.8992978487504288</v>
       </c>
       <c r="BJ20" t="n">
-        <v>0.9322687188161658</v>
+        <v>0.8992978487504288</v>
       </c>
       <c r="BK20" t="n">
-        <v>93.23</v>
+        <v>89.93000000000001</v>
       </c>
       <c r="BL20" t="inlineStr">
         <is>
@@ -4676,7 +4676,7 @@
         </is>
       </c>
       <c r="BM20" t="n">
-        <v>4.086234223136356</v>
+        <v>4.040287991549645</v>
       </c>
     </row>
     <row r="21">
@@ -5080,13 +5080,13 @@
         <v>0.4452126297784946</v>
       </c>
       <c r="BI22" t="n">
-        <v>0.9126564192645831</v>
+        <v>0.9366276693874802</v>
       </c>
       <c r="BJ22" t="n">
-        <v>0.9126564192645831</v>
+        <v>0.9366276693874802</v>
       </c>
       <c r="BK22" t="n">
-        <v>91.27</v>
+        <v>93.66</v>
       </c>
       <c r="BL22" t="inlineStr">
         <is>
@@ -5094,7 +5094,7 @@
         </is>
       </c>
       <c r="BM22" t="n">
-        <v>4.792711347074723</v>
+        <v>4.832155505921507</v>
       </c>
     </row>
   </sheetData>
@@ -5632,21 +5632,21 @@
         <v>0.6447590912226693</v>
       </c>
       <c r="BI2" t="n">
-        <v>0.4482987068515692</v>
+        <v>0.7435041105165291</v>
       </c>
       <c r="BJ2" t="n">
-        <v>0.4482987068515692</v>
+        <v>0.7435041105165291</v>
       </c>
       <c r="BK2" t="n">
-        <v>44.83</v>
+        <v>74.34999999999999</v>
       </c>
       <c r="BL2" t="inlineStr">
         <is>
-          <t>Aman</t>
+          <t>Terdampak</t>
         </is>
       </c>
       <c r="BM2" t="n">
-        <v>4.885981348578386</v>
+        <v>5.475112116106906</v>
       </c>
     </row>
     <row r="3">
@@ -5837,13 +5837,13 @@
         <v>0.584807660688538</v>
       </c>
       <c r="BI3" t="n">
-        <v>0.7804556995701294</v>
+        <v>0.7395082100789241</v>
       </c>
       <c r="BJ3" t="n">
-        <v>0.7804556995701294</v>
+        <v>0.7395082100789241</v>
       </c>
       <c r="BK3" t="n">
-        <v>78.05</v>
+        <v>73.95</v>
       </c>
       <c r="BL3" t="inlineStr">
         <is>
@@ -5851,7 +5851,7 @@
         </is>
       </c>
       <c r="BM3" t="n">
-        <v>3.874676683822134</v>
+        <v>3.817614712715328</v>
       </c>
     </row>
     <row r="4">
@@ -6041,13 +6041,13 @@
         <v>0.6928203230275504</v>
       </c>
       <c r="BI4" t="n">
-        <v>0.0001</v>
+        <v>0.251511556867749</v>
       </c>
       <c r="BJ4" t="n">
-        <v>0.0001</v>
+        <v>0.251511556867749</v>
       </c>
       <c r="BK4" t="n">
-        <v>0.01</v>
+        <v>25.15</v>
       </c>
       <c r="BL4" t="inlineStr">
         <is>
@@ -6247,13 +6247,13 @@
         <v>0.6328506932918696</v>
       </c>
       <c r="BI5" t="n">
-        <v>0.8660260372187892</v>
+        <v>0.8548821979343928</v>
       </c>
       <c r="BJ5" t="n">
-        <v>0.8660260372187892</v>
+        <v>0.8548821979343928</v>
       </c>
       <c r="BK5" t="n">
-        <v>86.59999999999999</v>
+        <v>85.48999999999999</v>
       </c>
       <c r="BL5" t="inlineStr">
         <is>
@@ -6261,7 +6261,7 @@
         </is>
       </c>
       <c r="BM5" t="n">
-        <v>3.993922385944024</v>
+        <v>3.978392998351124</v>
       </c>
     </row>
     <row r="6">
@@ -6453,13 +6453,13 @@
         <v>0.6026726190182244</v>
       </c>
       <c r="BI6" t="n">
-        <v>0.75847981791585</v>
+        <v>0.7139596494856451</v>
       </c>
       <c r="BJ6" t="n">
-        <v>0.75847981791585</v>
+        <v>0.7139596494856451</v>
       </c>
       <c r="BK6" t="n">
-        <v>75.84999999999999</v>
+        <v>71.40000000000001</v>
       </c>
       <c r="BL6" t="inlineStr">
         <is>
@@ -6467,7 +6467,7 @@
         </is>
       </c>
       <c r="BM6" t="n">
-        <v>5.753040698047799</v>
+        <v>5.660190157978803</v>
       </c>
     </row>
     <row r="7">
@@ -6868,13 +6868,13 @@
         <v>0.4452126297784946</v>
       </c>
       <c r="BI8" t="n">
-        <v>0.9126564192645831</v>
+        <v>0.9366276693874802</v>
       </c>
       <c r="BJ8" t="n">
-        <v>0.9126564192645831</v>
+        <v>0.9366276693874802</v>
       </c>
       <c r="BK8" t="n">
-        <v>91.27</v>
+        <v>93.66</v>
       </c>
       <c r="BL8" t="inlineStr">
         <is>
@@ -6882,7 +6882,7 @@
         </is>
       </c>
       <c r="BM8" t="n">
-        <v>4.792711347074723</v>
+        <v>4.832155505921507</v>
       </c>
     </row>
     <row r="9">
@@ -7074,13 +7074,13 @@
         <v>0</v>
       </c>
       <c r="BI9" t="n">
-        <v>0.9322687188161658</v>
+        <v>0.9259739153066067</v>
       </c>
       <c r="BJ9" t="n">
-        <v>0.9322687188161658</v>
+        <v>0.9259739153066067</v>
       </c>
       <c r="BK9" t="n">
-        <v>93.23</v>
+        <v>92.59999999999999</v>
       </c>
       <c r="BL9" t="inlineStr">
         <is>
@@ -7088,7 +7088,7 @@
         </is>
       </c>
       <c r="BM9" t="n">
-        <v>5.851822830711569</v>
+        <v>5.839260518582497</v>
       </c>
     </row>
     <row r="10">
@@ -7280,13 +7280,13 @@
         <v>0.6928203230275506</v>
       </c>
       <c r="BI10" t="n">
-        <v>0.06516278616970395</v>
+        <v>0.0001</v>
       </c>
       <c r="BJ10" t="n">
-        <v>0.06516278616970395</v>
+        <v>0.0001</v>
       </c>
       <c r="BK10" t="n">
-        <v>6.52</v>
+        <v>0.01</v>
       </c>
       <c r="BL10" t="inlineStr">
         <is>
@@ -7485,13 +7485,13 @@
         <v>0.4217311262607299</v>
       </c>
       <c r="BI11" t="n">
-        <v>0.8002671504870114</v>
+        <v>0.8626015846940868</v>
       </c>
       <c r="BJ11" t="n">
-        <v>0.8002671504870114</v>
+        <v>0.8626015846940868</v>
       </c>
       <c r="BK11" t="n">
-        <v>80.03</v>
+        <v>86.26000000000001</v>
       </c>
       <c r="BL11" t="inlineStr">
         <is>
@@ -7499,7 +7499,7 @@
         </is>
       </c>
       <c r="BM11" t="n">
-        <v>3.902284736326692</v>
+        <v>3.989150273820687</v>
       </c>
     </row>
     <row r="12">
@@ -7691,13 +7691,13 @@
         <v>0.707359274242687</v>
       </c>
       <c r="BI12" t="n">
-        <v>0.5635407836991131</v>
+        <v>0.5563274019391721</v>
       </c>
       <c r="BJ12" t="n">
-        <v>0.5635407836991131</v>
+        <v>0.5563274019391721</v>
       </c>
       <c r="BK12" t="n">
-        <v>56.35</v>
+        <v>55.63</v>
       </c>
       <c r="BL12" t="inlineStr">
         <is>
@@ -7705,7 +7705,7 @@
         </is>
       </c>
       <c r="BM12" t="n">
-        <v>5.115965801240466</v>
+        <v>5.101570315656695</v>
       </c>
     </row>
     <row r="13">
@@ -7898,13 +7898,13 @@
         <v>0.6244997998398401</v>
       </c>
       <c r="BI13" t="n">
-        <v>0.6775390761516846</v>
+        <v>0.6800692474526799</v>
       </c>
       <c r="BJ13" t="n">
-        <v>0.6775390761516846</v>
+        <v>0.6800692474526799</v>
       </c>
       <c r="BK13" t="n">
-        <v>67.75</v>
+        <v>68.01000000000001</v>
       </c>
       <c r="BL13" t="inlineStr">
         <is>
@@ -7912,7 +7912,7 @@
         </is>
       </c>
       <c r="BM13" t="n">
-        <v>3.296437275116855</v>
+        <v>3.299552281378881</v>
       </c>
     </row>
     <row r="14">
@@ -8105,13 +8105,13 @@
         <v>0.4777177887773147</v>
       </c>
       <c r="BI14" t="n">
-        <v>0.8449251380807483</v>
+        <v>0.8342082463533553</v>
       </c>
       <c r="BJ14" t="n">
-        <v>0.8449251380807483</v>
+        <v>0.8342082463533553</v>
       </c>
       <c r="BK14" t="n">
-        <v>84.48999999999999</v>
+        <v>83.42</v>
       </c>
       <c r="BL14" t="inlineStr">
         <is>
@@ -8119,7 +8119,7 @@
         </is>
       </c>
       <c r="BM14" t="n">
-        <v>5.933329653520449</v>
+        <v>5.910978678224625</v>
       </c>
     </row>
     <row r="15">
@@ -8311,13 +8311,13 @@
         <v>0.5457628998540878</v>
       </c>
       <c r="BI15" t="n">
-        <v>0.955342012406263</v>
+        <v>0.761243694776387</v>
       </c>
       <c r="BJ15" t="n">
-        <v>0.955342012406263</v>
+        <v>0.761243694776387</v>
       </c>
       <c r="BK15" t="n">
-        <v>95.53</v>
+        <v>76.12</v>
       </c>
       <c r="BL15" t="inlineStr">
         <is>
@@ -8325,7 +8325,7 @@
         </is>
       </c>
       <c r="BM15" t="n">
-        <v>4.118387784405595</v>
+        <v>3.847903983564655</v>
       </c>
     </row>
     <row r="16">
@@ -8517,13 +8517,13 @@
         <v>0.5855400437691201</v>
       </c>
       <c r="BI16" t="n">
-        <v>0.8233404440771093</v>
+        <v>0.9199718003314667</v>
       </c>
       <c r="BJ16" t="n">
-        <v>0.8233404440771093</v>
+        <v>0.9199718003314667</v>
       </c>
       <c r="BK16" t="n">
-        <v>82.33</v>
+        <v>92</v>
       </c>
       <c r="BL16" t="inlineStr">
         <is>
@@ -8531,7 +8531,7 @@
         </is>
       </c>
       <c r="BM16" t="n">
-        <v>3.934438297595932</v>
+        <v>4.069097973368776</v>
       </c>
     </row>
     <row r="17">
@@ -8724,13 +8724,13 @@
         <v>0</v>
       </c>
       <c r="BI17" t="n">
-        <v>1</v>
+        <v>0.8975343106629416</v>
       </c>
       <c r="BJ17" t="n">
-        <v>1</v>
+        <v>0.8975343106629416</v>
       </c>
       <c r="BK17" t="n">
-        <v>100</v>
+        <v>89.75</v>
       </c>
       <c r="BL17" t="inlineStr">
         <is>
@@ -8738,7 +8738,7 @@
         </is>
       </c>
       <c r="BM17" t="n">
-        <v>5.98699170355107</v>
+        <v>5.782504626231201</v>
       </c>
     </row>
     <row r="18">
@@ -8930,13 +8930,13 @@
         <v>0.630476010645922</v>
       </c>
       <c r="BI18" t="n">
-        <v>0.3884902514512227</v>
+        <v>0.5677565934530615</v>
       </c>
       <c r="BJ18" t="n">
-        <v>0.3884902514512227</v>
+        <v>0.5677565934530615</v>
       </c>
       <c r="BK18" t="n">
-        <v>38.85</v>
+        <v>56.78</v>
       </c>
       <c r="BL18" t="inlineStr">
         <is>
@@ -8944,7 +8944,7 @@
         </is>
       </c>
       <c r="BM18" t="n">
-        <v>4.766623773150359</v>
+        <v>5.124379140580679</v>
       </c>
     </row>
     <row r="19">
@@ -9136,13 +9136,13 @@
         <v>0.5185832348124723</v>
       </c>
       <c r="BI19" t="n">
-        <v>0.9322687188161658</v>
+        <v>0.8992978487504288</v>
       </c>
       <c r="BJ19" t="n">
-        <v>0.9322687188161658</v>
+        <v>0.8992978487504288</v>
       </c>
       <c r="BK19" t="n">
-        <v>93.23</v>
+        <v>89.93000000000001</v>
       </c>
       <c r="BL19" t="inlineStr">
         <is>
@@ -9150,7 +9150,7 @@
         </is>
       </c>
       <c r="BM19" t="n">
-        <v>4.086234223136356</v>
+        <v>4.040287991549645</v>
       </c>
     </row>
     <row r="20">
@@ -9551,13 +9551,13 @@
         <v>0.6026726190182213</v>
       </c>
       <c r="BI21" t="n">
-        <v>0.955342012406263</v>
+        <v>1</v>
       </c>
       <c r="BJ21" t="n">
-        <v>0.955342012406263</v>
+        <v>1</v>
       </c>
       <c r="BK21" t="n">
-        <v>95.53</v>
+        <v>100</v>
       </c>
       <c r="BL21" t="inlineStr">
         <is>
@@ -9565,7 +9565,7 @@
         </is>
       </c>
       <c r="BM21" t="n">
-        <v>4.36338906393521</v>
+        <v>4.429323962118182</v>
       </c>
     </row>
     <row r="22">
@@ -9757,13 +9757,13 @@
         <v>0.6579187965525378</v>
       </c>
       <c r="BI22" t="n">
-        <v>0.6546605430963264</v>
+        <v>0.6068919016003881</v>
       </c>
       <c r="BJ22" t="n">
-        <v>0.6546605430963264</v>
+        <v>0.6068919016003881</v>
       </c>
       <c r="BK22" t="n">
-        <v>65.47</v>
+        <v>60.69</v>
       </c>
       <c r="BL22" t="inlineStr">
         <is>
@@ -9771,7 +9771,7 @@
         </is>
       </c>
       <c r="BM22" t="n">
-        <v>5.297810215754027</v>
+        <v>5.202480062311999</v>
       </c>
     </row>
   </sheetData>
@@ -9785,7 +9785,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9801,84 +9801,36 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Best_Cost</t>
+          <t>PredictedBearing</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Node_Count</t>
+          <t>PredictedDistanceKM</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>PredictedLat</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>PredictedLon</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>PredictedBearing</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>PredictedDistanceKM</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
           <t>PredictedDirection</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>PredictedConfidence</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>MovementScale</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2025-12-29T23:33:19.736701</t>
+          <t>2025-12-30T18:12:07.355189</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>640515014540.4769</v>
+        <v>60.72043401770543</v>
       </c>
       <c r="C2" t="n">
-        <v>21</v>
-      </c>
-      <c r="D2" t="n">
-        <v>-7.994398215976737</v>
-      </c>
-      <c r="E2" t="n">
-        <v>114.2823584470765</v>
-      </c>
-      <c r="F2" t="n">
-        <v>93.51743294051084</v>
-      </c>
-      <c r="G2" t="n">
-        <v>7.982748640550591</v>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>E</t>
-        </is>
-      </c>
-      <c r="I2" t="n">
-        <v>0.4041904767157775</v>
-      </c>
-      <c r="J2" t="n">
-        <v>1.444660543096326</v>
+        <v>6.134758280905867</v>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>NE</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>